<commit_message>
new branch for tests before moving to master
</commit_message>
<xml_diff>
--- a/iluvanimals.xlsx
+++ b/iluvanimals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleychampagne/Documents/GitHub/GitHub-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7874FB3-2D02-EF4F-AA27-D696A71D2B57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B086682E-10ED-2B43-8473-D6B9BA54215F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{7E79456E-3B9B-874F-B1B5-BDA8C0E84262}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>dogs</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>birds</t>
+  </si>
+  <si>
+    <t>horses</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05ABDFB3-5DBF-F440-ABCE-ABAC3131FCE0}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -424,6 +427,11 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>